<commit_message>
[feature] finish write data
</commit_message>
<xml_diff>
--- a/My project/Excel2Config/Excel/Test1.xlsx
+++ b/My project/Excel2Config/Excel/Test1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\UnityProject\Auto_Excel_Reader\My project\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\UnityProject\Auto_Excel_Reader\My project\Excel2Config\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF699F7-4945-47EA-AA53-0352AC426ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0AB587-8E06-4FFE-83A8-1CC870DEB6CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10215" yWindow="2055" windowWidth="12135" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>ID</t>
   </si>
@@ -87,7 +87,19 @@
     <t>한국어</t>
   </si>
   <si>
-    <t>[12,163.5,90]</t>
+    <t>[12|163.5|90]</t>
+  </si>
+  <si>
+    <t>[[360.1|12|19],[96|1|56],[45|91.5|60]]</t>
+  </si>
+  <si>
+    <t>int[]</t>
+  </si>
+  <si>
+    <t>aaaaaa</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
   </si>
 </sst>
 </file>
@@ -424,15 +436,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -443,7 +455,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -465,8 +477,11 @@
       <c r="H2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -488,8 +503,11 @@
       <c r="H3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>100001</v>
       </c>
@@ -508,8 +526,14 @@
       <c r="F4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>100002</v>
       </c>
@@ -526,7 +550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>100003</v>
       </c>
@@ -543,7 +567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>100004</v>
       </c>
@@ -560,7 +584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>100005</v>
       </c>

</xml_diff>